<commit_message>
chore: Updated department module
</commit_message>
<xml_diff>
--- a/public/department_data.xlsx
+++ b/public/department_data.xlsx
@@ -427,13 +427,13 @@
         <v>B001</v>
       </c>
       <c r="C2" t="str">
-        <v>D001</v>
+        <v>DEP001</v>
       </c>
       <c r="D2" t="str">
         <v>Finance</v>
       </c>
       <c r="E2" t="str">
-        <v>finance department</v>
+        <v>division finance</v>
       </c>
     </row>
     <row r="3">
@@ -441,16 +441,16 @@
         <v>C001</v>
       </c>
       <c r="B3" t="str">
-        <v>B002</v>
+        <v>B001</v>
       </c>
       <c r="C3" t="str">
-        <v>D002</v>
+        <v>DEP002</v>
       </c>
       <c r="D3" t="str">
         <v>IT</v>
       </c>
       <c r="E3" t="str">
-        <v>it department</v>
+        <v>division it</v>
       </c>
     </row>
   </sheetData>

</xml_diff>